<commit_message>
actualizacion del modilo de planificacion territorial
</commit_message>
<xml_diff>
--- a/public/plantillas_territorial/plantilla_recursos.xlsx
+++ b/public/plantillas_territorial/plantilla_recursos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crisTerritorial\pipspie\public\plantillas_territorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pipspie\public\plantillas_territorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -330,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,13 +357,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,6 +419,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40:J40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,69 +728,69 @@
   <sheetData>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="27"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
@@ -801,353 +812,381 @@
       <c r="I6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
       <c r="B24" s="10"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="10"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="16"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="16"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="I37" s="33" t="s">
+      <c r="C37" s="29"/>
+      <c r="I37" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J37" s="33"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="33" t="s">
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="I38" s="33" t="s">
+      <c r="C38" s="29"/>
+      <c r="I38" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J38" s="33"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="33" t="s">
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="I39" s="33" t="s">
+      <c r="C39" s="29"/>
+      <c r="I39" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="33"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="33" t="s">
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
+      <c r="C40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>